<commit_message>
cleaned up  the formating on the params table and fixed some bigs
</commit_message>
<xml_diff>
--- a/extractorParametersExample.xlsx
+++ b/extractorParametersExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F1F5EDC4-EADE-4C06-8DB3-45CDB7A09728}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C14D8169-198F-4201-8795-35F1D21DED6D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" firstSheet="2" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
   </bookViews>
   <sheets>
     <sheet name="ExportDestinations" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="180">
   <si>
     <t>exportFolder</t>
   </si>
@@ -382,12 +382,213 @@
   <si>
     <t>\\server\LOCO.gdb\FocusAreas</t>
   </si>
+  <si>
+    <t>i.e. full path to the SDE DB or file GDB that contains the Geologic Map FDS</t>
+  </si>
+  <si>
+    <t>Just the name - not the full path</t>
+  </si>
+  <si>
+    <t>The number of characters in inputFDSName before "GeologicMap", don't include any characters before a period or the period itself (i.e. for SDE name ignore the stuff before the last period) - assumes a base name of "GeologicMap" consistent with GeMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: this polygon FC must have a string field called "Build". It should also have a "Type" of "31.31". At least one polygons needs to be flagged as Build "yes" (all lowercase). All the other FCs will be "clipped" to this polygon. </t>
+  </si>
+  <si>
+    <t>Note: these should be coma separated (spaces before or after the coma will be ignored)</t>
+  </si>
+  <si>
+    <t>Note: these should be coma separated (spaces before or after the coma will be ignored); instead of using clipping these features will be copied and parts outside the boundary will be deleted. This preserves feature linked annotations. It has only been tested with point FCs</t>
+  </si>
+  <si>
+    <t>Note: these should be coma separated (spaces before or after the coma will be ignored); this has only been tested with feature-linked annotations that are linked to the FCs in "listFCsToSelectByLocation"</t>
+  </si>
+  <si>
+    <t>The standalone GDB created will be named [this prefix]YEARMONTHDAY_HOUR_SECONDS</t>
+  </si>
+  <si>
+    <t>Note: To be GeMS compilant this should be left blank. Otherwise a prefix will be added to the FDS which is not allowed.</t>
+  </si>
+  <si>
+    <t>Do you want to build polygons from MapUnitPoints and ContactsAndFaults; if Yes type "True" if not "False" - nothing else; will be named "MapUnitPolys" per GeMs standards</t>
+  </si>
+  <si>
+    <t>Do want to remove a separate copy of the map boundary (the boundary will be in the contacts and faults as a neat lines); if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>Do you want to remove multi-part lines, which may be created by the process; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>Do you want to make some frequency tables; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>ignored if maleTables is "False"; listFCsForTables and listFieldsForTables must be the same length, coma separated (space before or after the coma are fine); consider adding the polygons created in buildPolygons to; these FCs must have been clipped into the standalone DB previously (see MainInputs lists)</t>
+  </si>
+  <si>
+    <t>Note: ignored if maleTables is "False"; listFCsForTables and listFieldsForTables must be the same length, coma separated (space before or after the coma are fine)</t>
+  </si>
+  <si>
+    <t>Do you want to null some fields; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>either "True" or "False" nothing else; this will "null" nonullable fields with -9999, #null, or # (You should have a very good reason for using this - avoid it if possible)</t>
+  </si>
+  <si>
+    <t>List of fields in each FC to null; ignored if null Fields is "False"; listFCsToNull and listFieldsToNull must be the same length, coma and "|" separated - separate fields in the same FC with "|" and FCs with comas (space before or after the coma are fine - no spaces between "|"s ??)</t>
+  </si>
+  <si>
+    <t>Do you want to drop unneeded field; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>Note: ignored if dropFields is "False"; listFCsToDropFldsFrom and listFieldsToDrop must be the same length, coma and "|" separated - separate fields in the same FC with "|" and FCs with comas (space before or after the coma are fine - no spaces between "|"s ??)</t>
+  </si>
+  <si>
+    <t>Do you want to add extra tables for some reason; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>The GDB that has the table you want to add</t>
+  </si>
+  <si>
+    <t>A coma separated list of the tables in that GDB to add</t>
+  </si>
+  <si>
+    <t>Do you want to add an arc version of the CMULMU; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>This should be "CorrelationOfMapUnits" or else it will not be GEMS compliant</t>
+  </si>
+  <si>
+    <t>The FDS with the CMU/LMU - everything will be copied over</t>
+  </si>
+  <si>
+    <t>Do you want to add a cross section to the database; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>This should be "CrossSectionA" or else it will not be GEMS compliant</t>
+  </si>
+  <si>
+    <t>The FDS with cross section A - everything will be copied over</t>
+  </si>
+  <si>
+    <t>Do you want to add another cross sections to the database; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>This should be "CrossSectionB" or else it will not be GEMS compliant</t>
+  </si>
+  <si>
+    <t>The FDS with cross section B - everything will be copied over</t>
+  </si>
+  <si>
+    <t>The FDS with cross section C - everything will be copied over</t>
+  </si>
+  <si>
+    <t>Do you want to add any other FCs from some other source; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>The FDS with the extra FCs</t>
+  </si>
+  <si>
+    <t>A coma separated list of the FCs to be copied</t>
+  </si>
+  <si>
+    <t>Do you want to add a DRG and clip it; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>Note: this has only been tested with Raster Mosaics</t>
+  </si>
+  <si>
+    <t>Do you want to exclude some line types from GeomorphLines; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>This is an SQL and everything else will be deleted from the exported FC</t>
+  </si>
+  <si>
+    <t>Do you want to exclude some orientation points; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>Do you want to want to rename all the fields in your DB; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t>If a field in the first column of this table is found it will be renamed what is in the second column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have to use an independent field you want to use to populate a series of dependent fields; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>Note instead of populating LTYPE or PTYPE we populate FGDC codes in the "Type" field. This code switches "Type" to "Symbol" and then populated other fields based on the "Symbol" field (We will likely switch it the future to just populating "Symbol" with FGDC codes). See the GeMS documentation on their Attribute By Key Values tool; a modified version of that tool (available on rcrow's github page) is used here</t>
+  </si>
+  <si>
+    <t>A coma sepatated list of feature classes that need "Type" and "Symbol" switched</t>
+  </si>
+  <si>
+    <t>This populates IndentityConfidence based on the presence of question marks in the mapunit field; if Yes type "True" if not "False" - nothing else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you need to change a field type; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>A coma separated list of the fields you want to change</t>
+  </si>
+  <si>
+    <t>The type you want to change it to; at this point all fields will be changed to the same thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to build a GeMS glossary from a master list of terms and definitions; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>This is a master table with types, defintions, and sources</t>
+  </si>
+  <si>
+    <t>This was created using the GeMS "Create New Database" tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to build a GeMS DataSource table from a master list of DataSources; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have FCs with DataSource information; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>A coma separated list of FC paths for FCs with DataSource information (see rcrow GitHub page for an example with the expected formating)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have excel tables with DataSource information; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>The path the the excel table with datasource information</t>
+  </si>
+  <si>
+    <t>A coma separated list of the fields which hold DataSource information (this should be everything in a GeMS DB)</t>
+  </si>
+  <si>
+    <t>A coma separated list of FCs that should be ignored when building the DataSources table</t>
+  </si>
+  <si>
+    <t>This writes a master DataSource excel table that combines all the FCs and tables that were input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to build topology; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>This assumes a series of desired rule related to a line FC that constrains the contacts and faults (this should not change for GEMS DBs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to use a modified version of the GeMS toolbox "(re)Set ID values" that was renamed to "Set ID Values" (you can download it from the rcrow GitHub site) to recalculate the _ID fields; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to use a modified version of the GeMS toolbox "Validate Databse" (you can download it from the rcrow GitHub site) to check if the resulting DB in GeMS compilant; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>List of FCs to null fields in; ignored if null Fields is "False"; listFCsToNull and listFieldsToNull must be the same length, coma separated (space before or after the coma are fine); these FCs must have been clipped into the standalone DB previously (see MainInputs lists); consider adding mapunit polygons if built</t>
+  </si>
+  <si>
+    <t>Note: ignored if dropFields is "False"; listFCsToDropFldsFrom and listFieldsToDrop must be the same length, coma separated; these FCs must have been clipped into the standalone DB previously (see MainInputs lists); consider adding mapunit polygons if built</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,53 +597,116 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FF008000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF0000FF"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -450,35 +714,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,37 +1154,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC125FBD-D0F5-4959-B8B0-FC41E4FBC2FA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="12" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C3" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -833,66 +1203,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FA449E-9BEE-4136-A080-9AE522277B5E}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="104.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="104.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C3" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>95</v>
       </c>
     </row>
@@ -904,472 +1298,660 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A77A94-9F3F-4811-816F-4015952F987C}">
-  <dimension ref="A1:BJ8"/>
+  <dimension ref="A1:BJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BP2" sqref="BP2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="125.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="150.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="3" customWidth="1"/>
-    <col min="19" max="19" width="86.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="86.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="86.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="86.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="150.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="75.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="78.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="94.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="23.42578125" style="3" customWidth="1"/>
-    <col min="49" max="49" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.42578125" style="3" customWidth="1"/>
-    <col min="51" max="51" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="84.85546875" style="3" customWidth="1"/>
-    <col min="53" max="53" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="38" style="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="33.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="18.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="125.140625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="18" customWidth="1"/>
+    <col min="18" max="18" width="30.5703125" style="18" customWidth="1"/>
+    <col min="19" max="19" width="54.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.7109375" style="18" customWidth="1"/>
+    <col min="22" max="22" width="54.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26" style="18" customWidth="1"/>
+    <col min="25" max="25" width="54.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24" style="18" customWidth="1"/>
+    <col min="28" max="28" width="54.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="47.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.140625" style="18" customWidth="1"/>
+    <col min="39" max="39" width="72.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.28515625" style="18" customWidth="1"/>
+    <col min="41" max="41" width="94.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="35.7109375" style="18" customWidth="1"/>
+    <col min="50" max="50" width="17.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="81" style="18" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="24.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="37.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="24.7109375" style="18" customWidth="1"/>
+    <col min="57" max="57" width="24.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="33.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="17.28515625" style="18" customWidth="1"/>
+    <col min="60" max="60" width="18.5703125" style="18" customWidth="1"/>
+    <col min="61" max="61" width="19.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="18.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:62" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF1" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL1" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN1" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO1" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP1" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="AQ1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AR1" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT1" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU1" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="AV1" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="AW1" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="AX1" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY1" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="AZ1" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="BA1" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="BB1" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="BC1" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BD1" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="BE1" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="BF1" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="BG1" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="BH1" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="BI1" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="BJ1" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AS2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AV2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AW2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AX2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AY2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BA2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BB2" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BC2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BD2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BE2" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BF2" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BG2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BH2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BI2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BJ2" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:62" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J3" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M3" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O3" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P3" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R3" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S3" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V3" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y3" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD3" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG3" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM3" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO3" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AP3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AS3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AT3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AU3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AV3" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AW3" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AX3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AY3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="AZ3" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BA3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="BB2" s="6" t="s">
+      <c r="BB3" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BC3" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BD3" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BE3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BF3" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BG3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="BH2" s="5" t="s">
+      <c r="BH3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BI3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="BJ2" s="3" t="s">
+      <c r="BJ3" s="18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="M4" s="7"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="M5" s="6"/>
+      <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="M6" s="7"/>
+      <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="M7" s="6"/>
+      <c r="M7" s="21"/>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="M8" s="7"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="M9" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added build DMU tool and fixed some bugs
</commit_message>
<xml_diff>
--- a/extractorParametersExample.xlsx
+++ b/extractorParametersExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CB89500F-BEFB-43E7-8484-2C09A09534E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3228B7AD-1F7A-48A7-AC9A-CECE1217675B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" firstSheet="2" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="204">
   <si>
     <t>exportFolder</t>
   </si>
@@ -615,6 +615,45 @@
   </si>
   <si>
     <t>DataSourceID|OrientationSourceID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to build a basic DMU; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>A master excel table with the DMU information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to null the Description field; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to null the AreaFillPatternDescription field; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to calculate the DescriptionOfMapUnits_ID; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to assign a single DescriptionSourceID to all the rows in the table; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>buildDMU</t>
+  </si>
+  <si>
+    <t>mapUnitTable</t>
+  </si>
+  <si>
+    <t>exampleBlankDMUTable</t>
+  </si>
+  <si>
+    <t>nullDescription</t>
+  </si>
+  <si>
+    <t>nullFillPattern</t>
+  </si>
+  <si>
+    <t>calculateIDs</t>
+  </si>
+  <si>
+    <t>descriptionSourceID</t>
   </si>
 </sst>
 </file>
@@ -739,7 +778,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -903,11 +942,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1019,6 +1069,9 @@
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1478,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A77A94-9F3F-4811-816F-4015952F987C}">
-  <dimension ref="A1:BN11"/>
+  <dimension ref="A1:BU11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AX3" sqref="AX3"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BQ3" sqref="BQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1606,7 @@
     <col min="67" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>122</v>
       </c>
@@ -1752,8 +1805,29 @@
       <c r="BN1" s="27" t="s">
         <v>176</v>
       </c>
+      <c r="BO1" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="BP1" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="BQ1" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BR1" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="BS1" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT1" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="BU1" s="17" t="s">
+        <v>196</v>
+      </c>
     </row>
-    <row r="2" spans="1:66" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:73" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
@@ -1952,8 +2026,29 @@
       <c r="BN2" s="25" t="s">
         <v>67</v>
       </c>
+      <c r="BO2" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="BP2" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="BQ2" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="BR2" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="BS2" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="BT2" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="BU2" s="24" t="s">
+        <v>203</v>
+      </c>
     </row>
-    <row r="3" spans="1:66" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>20</v>
       </c>
@@ -2152,26 +2247,35 @@
       <c r="BN3" s="40" t="s">
         <v>20</v>
       </c>
+      <c r="BO3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="BP3" s="36"/>
+      <c r="BQ3" s="36"/>
+      <c r="BR3" s="36"/>
+      <c r="BS3" s="36"/>
+      <c r="BT3" s="36"/>
+      <c r="BU3" s="36"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="M6" s="20"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="M8" s="20"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="M9" s="21"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E11" s="41"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting to ref toolbox more in standalone strip
</commit_message>
<xml_diff>
--- a/extractorParametersExample.xlsx
+++ b/extractorParametersExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3228B7AD-1F7A-48A7-AC9A-CECE1217675B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{362EAD19-3A91-4774-9AC2-2A9735697E4A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" firstSheet="2" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="ExportDestinations" sheetId="1" r:id="rId1"/>
     <sheet name="MainInputs" sheetId="3" r:id="rId2"/>
     <sheet name="InputsOptional" sheetId="2" r:id="rId3"/>
+    <sheet name="ToolPaths" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="210">
   <si>
     <t>exportFolder</t>
   </si>
@@ -654,6 +655,24 @@
   </si>
   <si>
     <t>descriptionSourceID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to populate the Label field based on the feature linked annotations; if Yes type "True" if not "False" - nothing else </t>
+  </si>
+  <si>
+    <t>populateLabelFromFeatureLinks</t>
+  </si>
+  <si>
+    <t>pathToGeMSToolB</t>
+  </si>
+  <si>
+    <t>pathToSchemaConvertToolB</t>
+  </si>
+  <si>
+    <t>\\server\folder\GeMS_ToolsArc10.tbx</t>
+  </si>
+  <si>
+    <t>\\server\folder\SchemaConvert.pyt</t>
   </si>
 </sst>
 </file>
@@ -957,7 +976,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1072,6 +1091,9 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A77A94-9F3F-4811-816F-4015952F987C}">
-  <dimension ref="A1:BU11"/>
+  <dimension ref="A1:BV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="BQ3" sqref="BQ3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1628,7 @@
     <col min="67" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>122</v>
       </c>
@@ -1823,11 +1845,14 @@
       <c r="BT1" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BU1" s="17" t="s">
+      <c r="BU1" s="26" t="s">
         <v>196</v>
       </c>
+      <c r="BV1" s="17" t="s">
+        <v>204</v>
+      </c>
     </row>
-    <row r="2" spans="1:73" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:74" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
@@ -2044,11 +2069,14 @@
       <c r="BT2" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="BU2" s="24" t="s">
+      <c r="BU2" s="30" t="s">
         <v>203</v>
       </c>
+      <c r="BV2" s="24" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="3" spans="1:73" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>20</v>
       </c>
@@ -2255,31 +2283,69 @@
       <c r="BR3" s="36"/>
       <c r="BS3" s="36"/>
       <c r="BT3" s="36"/>
-      <c r="BU3" s="36"/>
+      <c r="BU3" s="43"/>
+      <c r="BV3" s="36" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
       <c r="M6" s="20"/>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
       <c r="M8" s="20"/>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
       <c r="M9" s="21"/>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
       <c r="E11" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05709F78-EE2B-40E1-AC3E-33FF9F2FB7A3}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="80.28515625" customWidth="1"/>
+    <col min="2" max="2" width="90.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
converted one tool to two and added switch Type to Symbol standalone tool
</commit_message>
<xml_diff>
--- a/extractorParametersExample.xlsx
+++ b/extractorParametersExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{362EAD19-3A91-4774-9AC2-2A9735697E4A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F639FEA9-8897-41C3-9B03-4A889D2CC32F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" firstSheet="2" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" firstSheet="2" activeTab="3" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
   </bookViews>
   <sheets>
     <sheet name="ExportDestinations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="212">
   <si>
     <t>exportFolder</t>
   </si>
@@ -673,6 +673,12 @@
   </si>
   <si>
     <t>\\server\folder\SchemaConvert.pyt</t>
+  </si>
+  <si>
+    <t>pathToTableBuilderToolB</t>
+  </si>
+  <si>
+    <t>\\Igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\GeMSTableBuilder.pyt</t>
   </si>
 </sst>
 </file>
@@ -976,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1094,6 +1100,9 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1555,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A77A94-9F3F-4811-816F-4015952F987C}">
   <dimension ref="A1:BV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2317,10 +2326,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05709F78-EE2B-40E1-AC3E-33FF9F2FB7A3}">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,20 +2338,26 @@
     <col min="2" max="2" width="90.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>206</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>207</v>
       </c>
+      <c r="C2" s="44" t="s">
+        <v>210</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="150.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>208</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>209</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added an option to only populate SOME labels based on feature-linked annotations
</commit_message>
<xml_diff>
--- a/extractorParametersExample.xlsx
+++ b/extractorParametersExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Team\Crow\_Python\MapExtractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F639FEA9-8897-41C3-9B03-4A889D2CC32F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964492E2-CB7B-4FCC-9C0E-54F5DE9D8555}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5625" firstSheet="2" activeTab="3" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" firstSheet="2" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
   </bookViews>
   <sheets>
     <sheet name="ExportDestinations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="214">
   <si>
     <t>exportFolder</t>
   </si>
@@ -679,6 +679,12 @@
   </si>
   <si>
     <t>\\Igswzcwwgsrio\loco\Team\Crow\_Python\MapExtractor\GeMSTableBuilder.pyt</t>
+  </si>
+  <si>
+    <t>Do you want to keep the label field for specific annotation feature classes? If so put a coma seperated list of the annotation feature classes here</t>
+  </si>
+  <si>
+    <t>ignoreAnnos</t>
   </si>
 </sst>
 </file>
@@ -1562,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A77A94-9F3F-4811-816F-4015952F987C}">
-  <dimension ref="A1:BV11"/>
+  <dimension ref="A1:BW11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BV4" sqref="BV4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,7 +1643,7 @@
     <col min="67" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>122</v>
       </c>
@@ -1860,8 +1866,11 @@
       <c r="BV1" s="17" t="s">
         <v>204</v>
       </c>
+      <c r="BW1" s="17" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="2" spans="1:74" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:75" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
@@ -2084,8 +2093,11 @@
       <c r="BV2" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BW2" s="24" t="s">
+        <v>213</v>
+      </c>
     </row>
-    <row r="3" spans="1:74" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>20</v>
       </c>
@@ -2294,28 +2306,29 @@
       <c r="BT3" s="36"/>
       <c r="BU3" s="43"/>
       <c r="BV3" s="36" t="s">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="BW3" s="36"/>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="M6" s="20"/>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="M8" s="20"/>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="M9" s="21"/>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
       <c r="E11" s="41"/>
     </row>
   </sheetData>
@@ -2328,7 +2341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05709F78-EE2B-40E1-AC3E-33FF9F2FB7A3}">
   <dimension ref="A2:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Clipping is now an option
</commit_message>
<xml_diff>
--- a/extractorParametersExample.xlsx
+++ b/extractorParametersExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Team\Crow\_Python\MapExtractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964492E2-CB7B-4FCC-9C0E-54F5DE9D8555}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B9852A-85CF-45FF-AF92-F81D7CAEED5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" firstSheet="2" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" activeTab="2" xr2:uid="{E0B6631E-6032-4821-B1B0-3EDD50EBFBFE}"/>
   </bookViews>
   <sheets>
     <sheet name="ExportDestinations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="216">
   <si>
     <t>exportFolder</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t>ignoreAnnos</t>
+  </si>
+  <si>
+    <t>clip</t>
+  </si>
+  <si>
+    <t>If you want to clip the db to a map boundary type "True" is not type "False".</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1482,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,768 +1574,778 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A77A94-9F3F-4811-816F-4015952F987C}">
-  <dimension ref="A1:BW11"/>
+  <dimension ref="A1:BX11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="BV4" sqref="BV4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="125.140625" style="19" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="19" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" style="19" customWidth="1"/>
-    <col min="19" max="19" width="54.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.7109375" style="19" customWidth="1"/>
-    <col min="22" max="22" width="54.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26" style="19" customWidth="1"/>
-    <col min="25" max="25" width="54.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24" style="19" customWidth="1"/>
-    <col min="28" max="28" width="54.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="47.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.140625" style="19" customWidth="1"/>
-    <col min="39" max="39" width="72.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.28515625" style="19" customWidth="1"/>
-    <col min="41" max="41" width="94.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9" style="19" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="35.7109375" style="19" customWidth="1"/>
-    <col min="50" max="50" width="17.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="20.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="81" style="19" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="24.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="37.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24.7109375" style="19" customWidth="1"/>
-    <col min="57" max="57" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="33.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.28515625" style="19" customWidth="1"/>
-    <col min="60" max="60" width="18.5703125" style="19" customWidth="1"/>
-    <col min="61" max="61" width="19.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="18.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="63" max="65" width="9.140625" style="19"/>
-    <col min="66" max="66" width="18.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="19"/>
+    <col min="2" max="2" width="18.140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="125.140625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="19" customWidth="1"/>
+    <col min="19" max="19" width="30.5703125" style="19" customWidth="1"/>
+    <col min="20" max="20" width="54.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.7109375" style="19" customWidth="1"/>
+    <col min="23" max="23" width="54.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26" style="19" customWidth="1"/>
+    <col min="26" max="26" width="54.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24" style="19" customWidth="1"/>
+    <col min="29" max="29" width="54.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="47.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.140625" style="19" customWidth="1"/>
+    <col min="40" max="40" width="72.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.28515625" style="19" customWidth="1"/>
+    <col min="42" max="42" width="94.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9" style="19" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="35.7109375" style="19" customWidth="1"/>
+    <col min="51" max="51" width="17.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="81" style="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="24.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="37.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="24.7109375" style="19" customWidth="1"/>
+    <col min="58" max="58" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="33.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.28515625" style="19" customWidth="1"/>
+    <col min="61" max="61" width="18.5703125" style="19" customWidth="1"/>
+    <col min="62" max="62" width="19.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="18.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="64" max="66" width="9.140625" style="19"/>
+    <col min="67" max="67" width="18.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="68" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" s="17" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="T1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="X1" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="AA1" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AB1" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AE1" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AG1" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="AG1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="AH1" s="17" t="s">
+      <c r="AI1" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AI1" s="26" t="s">
+      <c r="AJ1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AJ1" s="17" t="s">
+      <c r="AK1" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="AK1" s="26" t="s">
+      <c r="AL1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AM1" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="AM1" s="26" t="s">
+      <c r="AN1" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AO1" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="AO1" s="17" t="s">
+      <c r="AP1" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="AP1" s="26" t="s">
+      <c r="AQ1" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="AQ1" s="17" t="s">
+      <c r="AR1" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="AR1" s="26" t="s">
+      <c r="AS1" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="AS1" s="27" t="s">
+      <c r="AT1" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="AT1" s="27" t="s">
+      <c r="AU1" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="AU1" s="17" t="s">
+      <c r="AV1" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="AV1" s="17" t="s">
+      <c r="AW1" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="AW1" s="26" t="s">
+      <c r="AX1" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="AX1" s="17" t="s">
+      <c r="AY1" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="AY1" s="17" t="s">
+      <c r="AZ1" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="AZ1" s="26" t="s">
+      <c r="BA1" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="BA1" s="17" t="s">
+      <c r="BB1" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="BB1" s="17" t="s">
+      <c r="BC1" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="BC1" s="17" t="s">
+      <c r="BD1" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="BD1" s="17" t="s">
+      <c r="BE1" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="BE1" s="17" t="s">
+      <c r="BF1" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="BF1" s="17" t="s">
+      <c r="BG1" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="BG1" s="17" t="s">
+      <c r="BH1" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="BH1" s="17" t="s">
+      <c r="BI1" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="BI1" s="17" t="s">
+      <c r="BJ1" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="BJ1" s="26" t="s">
+      <c r="BK1" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="BK1" s="17" t="s">
+      <c r="BL1" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="BL1" s="26" t="s">
+      <c r="BM1" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="BM1" s="27" t="s">
+      <c r="BN1" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="BN1" s="27" t="s">
+      <c r="BO1" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BO1" s="42" t="s">
+      <c r="BP1" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="BP1" s="17" t="s">
+      <c r="BQ1" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="BQ1" s="17" t="s">
+      <c r="BR1" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="BR1" s="17" t="s">
+      <c r="BS1" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="BS1" s="17" t="s">
+      <c r="BT1" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="BT1" s="17" t="s">
+      <c r="BU1" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BU1" s="26" t="s">
+      <c r="BV1" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="BV1" s="17" t="s">
+      <c r="BW1" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="BW1" s="17" t="s">
+      <c r="BX1" s="17" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:75" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" s="24" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="M2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="N2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="P2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="Q2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="T2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="U2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="V2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="22" t="s">
+      <c r="W2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="24" t="s">
+      <c r="Y2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="22" t="s">
+      <c r="Z2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="AA2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AB2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AB2" s="22" t="s">
+      <c r="AC2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AD2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="24" t="s">
+      <c r="AE2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AE2" s="30" t="s">
+      <c r="AF2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AF2" s="24" t="s">
+      <c r="AG2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AG2" s="22" t="s">
+      <c r="AH2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="24" t="s">
+      <c r="AI2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AI2" s="22" t="s">
+      <c r="AJ2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="24" t="s">
+      <c r="AK2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="22" t="s">
+      <c r="AL2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="24" t="s">
+      <c r="AM2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AM2" s="22" t="s">
+      <c r="AN2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="AN2" s="28" t="s">
+      <c r="AO2" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="AO2" s="28" t="s">
+      <c r="AP2" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="AP2" s="29" t="s">
+      <c r="AQ2" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="AQ2" s="24" t="s">
+      <c r="AR2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="AR2" s="22" t="s">
+      <c r="AS2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="AS2" s="23" t="s">
+      <c r="AT2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AT2" s="23" t="s">
+      <c r="AU2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AU2" s="24" t="s">
+      <c r="AV2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AV2" s="24" t="s">
+      <c r="AW2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AW2" s="22" t="s">
+      <c r="AX2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AX2" s="24" t="s">
+      <c r="AY2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AY2" s="24" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AZ2" s="22" t="s">
+      <c r="BA2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="BA2" s="24" t="s">
+      <c r="BB2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="BB2" s="24" t="s">
+      <c r="BC2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="BC2" s="24" t="s">
+      <c r="BD2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="BD2" s="18" t="s">
+      <c r="BE2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="BE2" s="24" t="s">
+      <c r="BF2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="BF2" s="24" t="s">
+      <c r="BG2" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="BG2" s="24" t="s">
+      <c r="BH2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="BH2" s="18" t="s">
+      <c r="BI2" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="BI2" s="24" t="s">
+      <c r="BJ2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="BJ2" s="30" t="s">
+      <c r="BK2" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="BK2" s="24" t="s">
+      <c r="BL2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="BL2" s="22" t="s">
+      <c r="BM2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="BM2" s="23" t="s">
+      <c r="BN2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BN2" s="25" t="s">
+      <c r="BO2" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="BO2" s="24" t="s">
+      <c r="BP2" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="BP2" s="24" t="s">
+      <c r="BQ2" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="BQ2" s="24" t="s">
+      <c r="BR2" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="BR2" s="24" t="s">
+      <c r="BS2" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="BS2" s="24" t="s">
+      <c r="BT2" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="BT2" s="24" t="s">
+      <c r="BU2" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="BU2" s="30" t="s">
+      <c r="BV2" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="BV2" s="24" t="s">
+      <c r="BW2" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BW2" s="24" t="s">
+      <c r="BX2" s="24" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:75" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="33" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="G3" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="J3" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="K3" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="N3" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="P3" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="Q3" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="S3" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="T3" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="V3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="W3" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="X3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="Y3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="Y3" s="32" t="s">
+      <c r="Z3" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="AA3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="AB3" s="32" t="s">
+      <c r="AC3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="AC3" s="19" t="s">
+      <c r="AD3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="19" t="s">
+      <c r="AE3" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AF3" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="AF3" s="19" t="s">
+      <c r="AG3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AG3" s="32" t="s">
+      <c r="AH3" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="AH3" s="19" t="s">
+      <c r="AI3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AI3" s="32" t="s">
+      <c r="AJ3" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="AJ3" s="19" t="s">
+      <c r="AK3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AK3" s="32" t="s">
+      <c r="AL3" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="AL3" s="19" t="s">
+      <c r="AM3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AM3" s="32" t="s">
+      <c r="AN3" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="AN3" s="36" t="s">
+      <c r="AO3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AO3" s="36" t="s">
+      <c r="AP3" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="AP3" s="37" t="s">
+      <c r="AQ3" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="AQ3" s="19" t="s">
+      <c r="AR3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AR3" s="19" t="s">
+      <c r="AS3" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="AS3" s="32" t="s">
+      <c r="AT3" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="AT3" s="33" t="s">
+      <c r="AU3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AU3" s="38" t="s">
+      <c r="AV3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="AV3" s="31" t="s">
+      <c r="AW3" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="AW3" s="32" t="s">
+      <c r="AX3" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="AX3" s="19" t="s">
+      <c r="AY3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AY3" s="19" t="s">
+      <c r="AZ3" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="AZ3" s="32" t="s">
+      <c r="BA3" s="32" t="s">
         <v>107</v>
-      </c>
-      <c r="BA3" s="19" t="s">
-        <v>20</v>
       </c>
       <c r="BB3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="31" t="s">
+      <c r="BC3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD3" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="BD3" s="19" t="s">
+      <c r="BE3" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="BE3" s="19" t="s">
+      <c r="BF3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="BF3" s="20" t="s">
+      <c r="BG3" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="BG3" s="19" t="s">
+      <c r="BH3" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="BH3" s="19" t="s">
+      <c r="BI3" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="BI3" s="19" t="s">
+      <c r="BJ3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="BJ3" s="32" t="s">
+      <c r="BK3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="BK3" s="19" t="s">
+      <c r="BL3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="BL3" s="39" t="s">
+      <c r="BM3" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="BM3" s="33" t="s">
+      <c r="BN3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="BN3" s="40" t="s">
+      <c r="BO3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="BO3" s="36" t="s">
+      <c r="BP3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="BP3" s="36"/>
       <c r="BQ3" s="36"/>
       <c r="BR3" s="36"/>
       <c r="BS3" s="36"/>
       <c r="BT3" s="36"/>
-      <c r="BU3" s="43"/>
-      <c r="BV3" s="36" t="s">
+      <c r="BU3" s="36"/>
+      <c r="BV3" s="43"/>
+      <c r="BW3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="BW3" s="36"/>
+      <c r="BX3" s="36"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="M4" s="20"/>
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="N4" s="20"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="M5" s="21"/>
+    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="M6" s="20"/>
+    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="N6" s="20"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="M7" s="21"/>
+    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="M8" s="20"/>
+    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="N8" s="20"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="M9" s="21"/>
+    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="N9" s="21"/>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="E11" s="41"/>
+    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="F11" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>